<commit_message>
Update documents and fix typos in English and Science materials; remove unused PDF file.
</commit_message>
<xml_diff>
--- a/pre primary oral marks slip/nursery/nur, orals.xlsx
+++ b/pre primary oral marks slip/nursery/nur, orals.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\2nd term exam 2082\pre primary oral marks slip\nursery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3538499-182B-4287-A84F-BBB3E7501648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B07300E-DB84-438E-BD75-D789E9231C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nur (Danfe)" sheetId="1" r:id="rId1"/>
     <sheet name="Nur (Dove)" sheetId="2" r:id="rId2"/>
+    <sheet name="Nur. (Dove) New" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
   <si>
     <t>Roll</t>
   </si>
@@ -219,6 +220,18 @@
   </si>
   <si>
     <t>Nur dove Nepali (O)</t>
+  </si>
+  <si>
+    <t>AADITYA NARAYAN SHRESTHA</t>
+  </si>
+  <si>
+    <t>JASBIKA SAI</t>
+  </si>
+  <si>
+    <t>DARSHAN BHUSAL</t>
+  </si>
+  <si>
+    <t>Nur. Dove Nepali (O)</t>
   </si>
 </sst>
 </file>
@@ -299,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,10 +330,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -650,10 +667,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="5">
         <v>1</v>
       </c>
@@ -703,7 +720,7 @@
       <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6"/>
@@ -720,7 +737,7 @@
       <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="6"/>
@@ -737,7 +754,7 @@
       <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="6"/>
@@ -754,7 +771,7 @@
       <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="6"/>
@@ -771,7 +788,7 @@
       <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="6"/>
@@ -788,7 +805,7 @@
       <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="6"/>
@@ -805,7 +822,7 @@
       <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="6"/>
@@ -822,7 +839,7 @@
       <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="6"/>
@@ -839,7 +856,7 @@
       <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="6"/>
@@ -856,7 +873,7 @@
       <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="6"/>
@@ -873,7 +890,7 @@
       <c r="A13" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="6"/>
@@ -890,7 +907,7 @@
       <c r="A14" s="7">
         <v>11</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="6"/>
@@ -907,7 +924,7 @@
       <c r="A15" s="7">
         <v>12</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="6"/>
@@ -924,7 +941,7 @@
       <c r="A16" s="7">
         <v>13</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="6"/>
@@ -941,7 +958,7 @@
       <c r="A17" s="7">
         <v>14</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="6"/>
@@ -958,7 +975,7 @@
       <c r="A18" s="7">
         <v>15</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="6"/>
@@ -975,7 +992,7 @@
       <c r="A19" s="7">
         <v>16</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="6"/>
@@ -992,7 +1009,7 @@
       <c r="A20" s="7">
         <v>17</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="6"/>
@@ -1009,7 +1026,7 @@
       <c r="A21" s="7">
         <v>18</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="6"/>
@@ -1026,7 +1043,7 @@
       <c r="A22" s="7">
         <v>19</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="6"/>
@@ -1043,7 +1060,7 @@
       <c r="A23" s="7">
         <v>20</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="6"/>
@@ -1060,7 +1077,7 @@
       <c r="A24" s="7">
         <v>21</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="6"/>
@@ -1077,7 +1094,7 @@
       <c r="A25" s="7">
         <v>22</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="6"/>
@@ -1094,7 +1111,7 @@
       <c r="A26" s="7">
         <v>23</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="6"/>
@@ -1111,7 +1128,7 @@
       <c r="A27" s="7">
         <v>24</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="6"/>
@@ -1128,7 +1145,7 @@
       <c r="A28" s="7">
         <v>25</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="6"/>
@@ -1145,7 +1162,7 @@
       <c r="A29" s="7">
         <v>26</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="6"/>
@@ -1162,7 +1179,7 @@
       <c r="A30" s="7">
         <v>27</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="6"/>
@@ -1179,7 +1196,7 @@
       <c r="A31" s="7">
         <v>28</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="6"/>
@@ -1205,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B05B460-024F-4976-BC35-94464D40DD78}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection sqref="A1:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="15"/>
@@ -1218,10 +1235,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="5">
         <v>1</v>
       </c>
@@ -1835,4 +1852,665 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9282C8-B0CC-4101-A159-2157F99CBC8D}">
+  <dimension ref="A1:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75">
+      <c r="A1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="5">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="10">
+        <v>26</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="10">
+        <v>29</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="10">
+        <v>30</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="10">
+        <v>31</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="10">
+        <v>32</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" s="16" customFormat="1">
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+    </row>
+    <row r="35" spans="1:12" s="16" customFormat="1">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update nursery oral marks spreadsheet
</commit_message>
<xml_diff>
--- a/pre primary oral marks slip/nursery/nur, orals.xlsx
+++ b/pre primary oral marks slip/nursery/nur, orals.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\2nd term exam 2082\pre primary oral marks slip\nursery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B07300E-DB84-438E-BD75-D789E9231C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20ADE61A-D3DC-41F8-835D-7C1312E27DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nur (Danfe)" sheetId="1" r:id="rId1"/>
-    <sheet name="Nur (Dove)" sheetId="2" r:id="rId2"/>
-    <sheet name="Nur. (Dove) New" sheetId="3" r:id="rId3"/>
+    <sheet name="Nur. (Dove) New" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Roll</t>
   </si>
@@ -141,9 +140,6 @@
     <t>SANVI CHAUDHARY</t>
   </si>
   <si>
-    <t>SAANVI CHAUDHARY</t>
-  </si>
-  <si>
     <t>RIYASA MAHATO</t>
   </si>
   <si>
@@ -156,9 +152,6 @@
     <t>PRIYANS MAHATO</t>
   </si>
   <si>
-    <t>PRAVESH TAMANG</t>
-  </si>
-  <si>
     <t>NEMAT KHATUN</t>
   </si>
   <si>
@@ -177,18 +170,12 @@
     <t>KARTIK THAKUR</t>
   </si>
   <si>
-    <t>KARTIK CHAUDHARY</t>
-  </si>
-  <si>
     <t>JERUSHA SUNAR</t>
   </si>
   <si>
     <t>HIMANI TAMANG</t>
   </si>
   <si>
-    <t>ELAZNA CHAUDHARY</t>
-  </si>
-  <si>
     <t>DIBINSH CHAUDHARY</t>
   </si>
   <si>
@@ -213,15 +200,6 @@
     <t>AAILA RAI</t>
   </si>
   <si>
-    <t>AADITYA NARAYANI SHRESTHA</t>
-  </si>
-  <si>
-    <t>Nur (Danfe), Nepali (O)</t>
-  </si>
-  <si>
-    <t>Nur dove Nepali (O)</t>
-  </si>
-  <si>
     <t>AADITYA NARAYAN SHRESTHA</t>
   </si>
   <si>
@@ -231,7 +209,10 @@
     <t>DARSHAN BHUSAL</t>
   </si>
   <si>
-    <t>Nur. Dove Nepali (O)</t>
+    <t>Nur. Dove Rhymes &amp; Conv.</t>
+  </si>
+  <si>
+    <t>Nur (Danfe), Rhymes &amp; Conv.</t>
   </si>
 </sst>
 </file>
@@ -312,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -335,9 +316,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,25 +634,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="11" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="12" width="10" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75">
-      <c r="A1" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="12"/>
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75">
+      <c r="A1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="15"/>
       <c r="C1" s="5">
         <v>1</v>
       </c>
@@ -698,8 +681,11 @@
       <c r="K1" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -715,8 +701,9 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75">
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -732,8 +719,9 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75">
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -749,8 +737,9 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75">
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -766,8 +755,9 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75">
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -783,8 +773,9 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75">
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -800,8 +791,9 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75">
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -817,8 +809,9 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75">
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -834,8 +827,9 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75">
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -851,8 +845,9 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -868,8 +863,9 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75">
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -885,8 +881,9 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75">
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -902,8 +899,9 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75">
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -919,8 +917,9 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75">
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -936,8 +935,9 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75">
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -953,8 +953,9 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75">
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -970,8 +971,9 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75">
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -987,8 +989,9 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75">
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -1004,8 +1007,9 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75">
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -1021,8 +1025,9 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -1038,8 +1043,9 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75">
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="7">
         <v>19</v>
       </c>
@@ -1055,8 +1061,9 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75">
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -1072,8 +1079,9 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75">
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="7">
         <v>21</v>
       </c>
@@ -1089,8 +1097,9 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75">
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -1106,8 +1115,9 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75">
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="7">
         <v>23</v>
       </c>
@@ -1123,8 +1133,9 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75">
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="7">
         <v>24</v>
       </c>
@@ -1140,8 +1151,9 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75">
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="7">
         <v>25</v>
       </c>
@@ -1157,8 +1169,9 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75">
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75">
       <c r="A29" s="7">
         <v>26</v>
       </c>
@@ -1174,8 +1187,9 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75">
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="7">
         <v>27</v>
       </c>
@@ -1191,8 +1205,9 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75">
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75">
       <c r="A31" s="7">
         <v>28</v>
       </c>
@@ -1208,6 +1223,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1219,26 +1235,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B05B460-024F-4976-BC35-94464D40DD78}">
-  <dimension ref="A1:K35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9282C8-B0CC-4101-A159-2157F99CBC8D}">
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:L35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="11.140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="4.5703125" style="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="12"/>
+    <row r="1" spans="1:12" ht="15.75">
+      <c r="A1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="15"/>
       <c r="C1" s="5">
         <v>1</v>
       </c>
@@ -1266,8 +1280,11 @@
       <c r="K1" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L1" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1283,13 +1300,14 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>63</v>
+      <c r="B3" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1300,13 +1318,14 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>62</v>
+      <c r="B4" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -1317,13 +1336,14 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>61</v>
+      <c r="B5" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1334,13 +1354,14 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>60</v>
+      <c r="B6" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1351,13 +1372,14 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>59</v>
+      <c r="B7" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -1368,13 +1390,14 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>58</v>
+      <c r="B8" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -1385,13 +1408,14 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>57</v>
+      <c r="B9" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1402,13 +1426,14 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>56</v>
+      <c r="B10" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -1419,13 +1444,14 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>55</v>
+      <c r="B11" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1436,13 +1462,14 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>54</v>
+      <c r="B12" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1453,13 +1480,14 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>53</v>
+      <c r="B13" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1470,13 +1498,14 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>52</v>
+      <c r="B14" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1487,13 +1516,14 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>51</v>
+      <c r="B15" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1504,13 +1534,14 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>50</v>
+      <c r="B16" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1521,13 +1552,14 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>49</v>
+      <c r="B17" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1538,13 +1570,14 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>48</v>
+      <c r="B18" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1555,13 +1588,14 @@
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>47</v>
+      <c r="B19" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1572,13 +1606,14 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>46</v>
+      <c r="B20" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1589,13 +1624,14 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>45</v>
+      <c r="B21" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -1606,13 +1642,14 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>44</v>
+      <c r="B22" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -1623,13 +1660,14 @@
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>43</v>
+      <c r="B23" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -1640,13 +1678,14 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>42</v>
+      <c r="B24" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1657,13 +1696,14 @@
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="10">
         <v>24</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>41</v>
+      <c r="B25" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -1674,13 +1714,14 @@
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="10">
         <v>25</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>40</v>
+      <c r="B26" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -1691,13 +1732,14 @@
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>39</v>
+      <c r="B27" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -1708,13 +1750,14 @@
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>38</v>
+      <c r="B28" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1725,13 +1768,14 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-    </row>
-    <row r="29" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>37</v>
+      <c r="B29" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1742,13 +1786,14 @@
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
-    </row>
-    <row r="30" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>36</v>
+      <c r="B30" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1759,13 +1804,14 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-    </row>
-    <row r="31" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L30" s="9"/>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="10">
         <v>30</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>35</v>
+      <c r="B31" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -1776,13 +1822,14 @@
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>34</v>
+      <c r="B32" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1793,13 +1840,14 @@
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>33</v>
+      <c r="B33" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -1810,701 +1858,35 @@
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
-    </row>
-    <row r="34" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A34" s="10">
-        <v>33</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-    </row>
-    <row r="35" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A35" s="10">
-        <v>34</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9282C8-B0CC-4101-A159-2157F99CBC8D}">
-  <dimension ref="A1:L35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="5">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5">
-        <v>5</v>
-      </c>
-      <c r="H1" s="5">
-        <v>6</v>
-      </c>
-      <c r="I1" s="5">
-        <v>7</v>
-      </c>
-      <c r="J1" s="5">
-        <v>8</v>
-      </c>
-      <c r="K1" s="5">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="10">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="10">
-        <v>11</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="10">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="10">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="10">
-        <v>14</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="10">
-        <v>15</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="10">
-        <v>16</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="10">
-        <v>17</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="10">
-        <v>18</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="10">
-        <v>19</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="10">
-        <v>20</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="10">
-        <v>21</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="10">
-        <v>22</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="10">
-        <v>23</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="10">
-        <v>24</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="10">
-        <v>25</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="10">
-        <v>26</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="10">
-        <v>27</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="10">
-        <v>28</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="10">
-        <v>29</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="10">
-        <v>30</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="10">
-        <v>31</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="10">
-        <v>32</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:12" s="16" customFormat="1">
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="14"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-    </row>
-    <row r="35" spans="1:12" s="16" customFormat="1">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="14"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>